<commit_message>
Updated run plan in Samples spreadsheet
</commit_message>
<xml_diff>
--- a/Samples.xlsx
+++ b/Samples.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NSRL15A" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="237">
   <si>
     <t>Irradiation 1, Front</t>
   </si>
@@ -174,16 +174,10 @@
     <t>014B_C100_2</t>
   </si>
   <si>
-    <t>100A_C100_1</t>
-  </si>
-  <si>
-    <t>100A_C100_2</t>
-  </si>
-  <si>
-    <t>100B_C100_1</t>
-  </si>
-  <si>
-    <t>100B_C100_2</t>
+    <t>100_C100_1</t>
+  </si>
+  <si>
+    <t>100_C100_2</t>
   </si>
   <si>
     <t>F_C100_1</t>
@@ -240,16 +234,10 @@
     <t>014B_C1000_2</t>
   </si>
   <si>
-    <t>100A_C1000_1</t>
-  </si>
-  <si>
-    <t>100A_C1000_2</t>
-  </si>
-  <si>
-    <t>100B_C1000_1</t>
-  </si>
-  <si>
-    <t>100B_C1000_2</t>
+    <t>100_C1000_1</t>
+  </si>
+  <si>
+    <t>100_C1000_2</t>
   </si>
   <si>
     <t>PP_C2000_1</t>
@@ -300,16 +288,10 @@
     <t>014B_C2000_2</t>
   </si>
   <si>
-    <t>100A_C2000_1</t>
-  </si>
-  <si>
-    <t>100A_C2000_2</t>
-  </si>
-  <si>
-    <t>100B_C2000_1</t>
-  </si>
-  <si>
-    <t>100B_C2000_2</t>
+    <t>100_C2000_1</t>
+  </si>
+  <si>
+    <t>100_C2000_2</t>
   </si>
   <si>
     <t>PP_C200_1</t>
@@ -438,12 +420,6 @@
     <t>100_R35_REF</t>
   </si>
   <si>
-    <t>005A_PMT1_REF</t>
-  </si>
-  <si>
-    <t>005A_PMT2_REF</t>
-  </si>
-  <si>
     <t>CERF Tray</t>
   </si>
   <si>
@@ -498,16 +474,10 @@
     <t>014B_C100_2_REF</t>
   </si>
   <si>
-    <t>100A_C100_1_REF</t>
-  </si>
-  <si>
-    <t>100A_C100_2_REF</t>
-  </si>
-  <si>
-    <t>100B_C100_1_REF</t>
-  </si>
-  <si>
-    <t>100B_C100_2_REF</t>
+    <t>100_C100_1_REF</t>
+  </si>
+  <si>
+    <t>100_C100_2_REF</t>
   </si>
   <si>
     <t>PP_C1000_1_REF</t>
@@ -558,16 +528,10 @@
     <t>014B_C1000_2_REF</t>
   </si>
   <si>
-    <t>100A_C1000_1_REF</t>
-  </si>
-  <si>
-    <t>100A_C1000_2_REF</t>
-  </si>
-  <si>
-    <t>100B_C1000_1_REF</t>
-  </si>
-  <si>
-    <t>100B_C1000_2_REF</t>
+    <t>100_C1000_1_REF</t>
+  </si>
+  <si>
+    <t>100_C1000_2_REF</t>
   </si>
   <si>
     <t>PP_C2000_1_REF</t>
@@ -618,16 +582,10 @@
     <t>014B_C2000_2_REF</t>
   </si>
   <si>
-    <t>100A_C2000_1_REF</t>
-  </si>
-  <si>
-    <t>100A_C2000_2_REF</t>
-  </si>
-  <si>
-    <t>100B_C2000_1_REF</t>
-  </si>
-  <si>
-    <t>100B_C2000_2_REF</t>
+    <t>100_C2000_1_REF</t>
+  </si>
+  <si>
+    <t>100_C2000_2_REF</t>
   </si>
   <si>
     <t>PP_C200_1_REF</t>
@@ -904,15 +862,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -924,11 +882,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1534,7 +1492,7 @@
       <c r="D16" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="0" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1554,11 +1512,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1568,10 +1526,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1662,12 +1620,6 @@
       <c r="V2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="W2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1677,64 +1629,58 @@
         <v>61.7</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="S3" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="T3" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,64 +1691,58 @@
         <v>38.5</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="L4" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="Q4" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="S4" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="T4" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,16 +1753,16 @@
         <v>159.3</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,16 +1773,16 @@
         <v>107.6</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,16 +1793,16 @@
         <v>84.6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,25 +1813,25 @@
         <v>71</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1914,39 +1854,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1958,8 +1898,8 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1973,12 +1913,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -2015,76 +1955,76 @@
       <c r="A3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="str">
+      <c r="B3" s="4" t="str">
         <f aca="false">NSRL15A!D3</f>
         <v>005A_F13</v>
       </c>
-      <c r="C3" s="5" t="str">
+      <c r="C3" s="4" t="str">
         <f aca="false">NSRL15A!E3</f>
         <v>005A_F14</v>
       </c>
-      <c r="D3" s="5" t="str">
+      <c r="D3" s="4" t="str">
         <f aca="false">NSRL15A!F3</f>
         <v>010A_F15</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>125</v>
+      <c r="E3" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="str">
+      <c r="B4" s="4" t="str">
         <f aca="false">NSRL15A!D4</f>
         <v>014A_F23</v>
       </c>
-      <c r="C4" s="5" t="str">
+      <c r="C4" s="4" t="str">
         <f aca="false">NSRL15A!E4</f>
         <v>F_F24</v>
       </c>
-      <c r="D4" s="5" t="str">
+      <c r="D4" s="4" t="str">
         <f aca="false">NSRL15A!F4</f>
         <v>010A_F25</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>126</v>
+      <c r="E4" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
-        <v>127</v>
+      <c r="G4" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="str">
+      <c r="B5" s="4" t="str">
         <f aca="false">NSRL15A!D5</f>
         <v>014A_F33</v>
       </c>
-      <c r="C5" s="5" t="str">
+      <c r="C5" s="4" t="str">
         <f aca="false">NSRL15A!E5</f>
         <v>100_F34</v>
       </c>
-      <c r="D5" s="5" t="str">
+      <c r="D5" s="4" t="str">
         <f aca="false">NSRL15A!F5</f>
         <v>100_F35</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>130</v>
+      <c r="E5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,14 +2043,14 @@
         <f aca="false">NSRL15A!O3</f>
         <v>010A_R15</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>133</v>
+      <c r="E6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,12 +2069,12 @@
         <f aca="false">NSRL15A!O4</f>
         <v>010A_R25</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>134</v>
+      <c r="E7" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
-        <v>135</v>
+      <c r="G7" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,14 +2093,14 @@
         <f aca="false">NSRL15A!O5</f>
         <v>100_R35</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>138</v>
+      <c r="E8" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,18 +2111,17 @@
         <f aca="false">NSRL15A!B16</f>
         <v>005A_PMT1</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>139</v>
-      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="str">
+      <c r="B10" s="9" t="str">
         <f aca="false">NSRL15A!B17</f>
         <v>F_PMT1</v>
       </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2192,27 +2131,33 @@
         <f aca="false">NSRL15A!E16</f>
         <v>005A_PMT2</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>140</v>
-      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="10" t="str">
+      <c r="B12" s="9" t="str">
         <f aca="false">NSRL15A!E17</f>
         <v>F_PMT2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">8+10+8+10+8+10+6+4</f>
+        <v>64</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">B15*2</f>
+        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0</v>
@@ -2249,43 +2194,43 @@
       <c r="A17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B17" s="5" t="str">
+      <c r="B17" s="4" t="str">
         <f aca="false">'CERF Run'!C2</f>
         <v>PP_C100_1</v>
       </c>
-      <c r="C17" s="5" t="str">
+      <c r="C17" s="4" t="str">
         <f aca="false">'CERF Run'!D2</f>
         <v>PP_C100_2</v>
       </c>
-      <c r="D17" s="5" t="str">
+      <c r="D17" s="4" t="str">
         <f aca="false">'CERF Run'!E2</f>
         <v>HDPE_C100_1</v>
       </c>
-      <c r="E17" s="5" t="str">
+      <c r="E17" s="4" t="str">
         <f aca="false">'CERF Run'!F2</f>
         <v>HDPE_C100_2</v>
       </c>
-      <c r="F17" s="5" t="str">
+      <c r="F17" s="4" t="str">
         <f aca="false">'CERF Run'!G2</f>
         <v>005A_C100_1</v>
       </c>
-      <c r="G17" s="5" t="str">
+      <c r="G17" s="4" t="str">
         <f aca="false">'CERF Run'!H2</f>
         <v>005A_C100_2</v>
       </c>
-      <c r="H17" s="5" t="str">
+      <c r="H17" s="4" t="str">
         <f aca="false">'CERF Run'!I2</f>
         <v>005B_C100_1</v>
       </c>
-      <c r="I17" s="5" t="str">
+      <c r="I17" s="4" t="str">
         <f aca="false">'CERF Run'!J2</f>
         <v>005B_C100_2</v>
       </c>
-      <c r="J17" s="5" t="str">
+      <c r="J17" s="4" t="str">
         <f aca="false">'CERF Run'!K2</f>
         <v>010A_C100_1</v>
       </c>
-      <c r="K17" s="5" t="str">
+      <c r="K17" s="4" t="str">
         <f aca="false">'CERF Run'!L2</f>
         <v>010A_C100_2</v>
       </c>
@@ -2294,305 +2239,281 @@
       <c r="A18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="5" t="str">
+      <c r="B18" s="4" t="str">
         <f aca="false">'CERF Run'!M2</f>
         <v>010B_C100_1</v>
       </c>
-      <c r="C18" s="5" t="str">
+      <c r="C18" s="4" t="str">
         <f aca="false">'CERF Run'!N2</f>
         <v>010B_C100_2</v>
       </c>
-      <c r="D18" s="5" t="str">
+      <c r="D18" s="4" t="str">
         <f aca="false">'CERF Run'!O2</f>
         <v>014A_C100_1</v>
       </c>
-      <c r="E18" s="5" t="str">
+      <c r="E18" s="4" t="str">
         <f aca="false">'CERF Run'!P2</f>
         <v>014A_C100_2</v>
       </c>
-      <c r="F18" s="5" t="str">
+      <c r="F18" s="4" t="str">
         <f aca="false">'CERF Run'!Q2</f>
         <v>014B_C100_1</v>
       </c>
-      <c r="G18" s="5" t="str">
+      <c r="G18" s="4" t="str">
         <f aca="false">'CERF Run'!R2</f>
         <v>014B_C100_2</v>
       </c>
-      <c r="H18" s="5" t="str">
+      <c r="H18" s="4" t="str">
         <f aca="false">'CERF Run'!S2</f>
-        <v>100A_C100_1</v>
-      </c>
-      <c r="I18" s="5" t="str">
+        <v>100_C100_1</v>
+      </c>
+      <c r="I18" s="4" t="str">
         <f aca="false">'CERF Run'!T2</f>
-        <v>100A_C100_2</v>
-      </c>
-      <c r="J18" s="5" t="str">
+        <v>100_C100_2</v>
+      </c>
+      <c r="J18" s="4" t="str">
         <f aca="false">'CERF Run'!U2</f>
-        <v>100B_C100_1</v>
-      </c>
-      <c r="K18" s="5" t="str">
+        <v>F_C100_1</v>
+      </c>
+      <c r="K18" s="4" t="str">
         <f aca="false">'CERF Run'!V2</f>
-        <v>100B_C100_2</v>
+        <v>F_C100_2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B19" s="5" t="str">
-        <f aca="false">'CERF Run'!W2</f>
-        <v>F_C100_1</v>
-      </c>
-      <c r="C19" s="5" t="str">
-        <f aca="false">'CERF Run'!X2</f>
-        <v>F_C100_2</v>
-      </c>
-      <c r="D19" s="7" t="str">
+      <c r="B19" s="7" t="str">
         <f aca="false">'CERF Run'!C3</f>
         <v>PP_C1000_1</v>
       </c>
-      <c r="E19" s="7" t="str">
+      <c r="C19" s="7" t="str">
         <f aca="false">'CERF Run'!D3</f>
         <v>PP_C1000_2</v>
       </c>
-      <c r="F19" s="7" t="str">
+      <c r="D19" s="7" t="str">
         <f aca="false">'CERF Run'!E3</f>
         <v>HDPE_C1000_1</v>
       </c>
-      <c r="G19" s="7" t="str">
+      <c r="E19" s="7" t="str">
         <f aca="false">'CERF Run'!F3</f>
         <v>HDPE_C1000_2</v>
       </c>
-      <c r="H19" s="7" t="str">
+      <c r="F19" s="7" t="str">
         <f aca="false">'CERF Run'!G3</f>
         <v>005A_C1000_1</v>
       </c>
-      <c r="I19" s="7" t="str">
+      <c r="G19" s="7" t="str">
         <f aca="false">'CERF Run'!H3</f>
         <v>005A_C1000_2</v>
       </c>
-      <c r="J19" s="7" t="str">
+      <c r="H19" s="7" t="str">
         <f aca="false">'CERF Run'!I3</f>
         <v>005B_C1000_1</v>
       </c>
-      <c r="K19" s="7" t="str">
+      <c r="I19" s="7" t="str">
         <f aca="false">'CERF Run'!J3</f>
         <v>005B_C1000_2</v>
       </c>
+      <c r="J19" s="7" t="str">
+        <f aca="false">'CERF Run'!K3</f>
+        <v>010A_C1000_1</v>
+      </c>
+      <c r="K19" s="7" t="str">
+        <f aca="false">'CERF Run'!L3</f>
+        <v>010A_C1000_2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B20" s="7" t="str">
-        <f aca="false">'CERF Run'!K3</f>
-        <v>010A_C1000_1</v>
-      </c>
-      <c r="C20" s="7" t="str">
-        <f aca="false">'CERF Run'!L3</f>
-        <v>010A_C1000_2</v>
-      </c>
-      <c r="D20" s="7" t="str">
         <f aca="false">'CERF Run'!M3</f>
         <v>010B_C1000_1</v>
       </c>
-      <c r="E20" s="7" t="str">
+      <c r="C20" s="7" t="str">
         <f aca="false">'CERF Run'!N3</f>
         <v>010B_C1000_2</v>
       </c>
-      <c r="F20" s="7" t="str">
+      <c r="D20" s="7" t="str">
         <f aca="false">'CERF Run'!O3</f>
         <v>014A_C1000_1</v>
       </c>
-      <c r="G20" s="7" t="str">
+      <c r="E20" s="7" t="str">
         <f aca="false">'CERF Run'!P3</f>
         <v>014A_C1000_2</v>
       </c>
-      <c r="H20" s="7" t="str">
+      <c r="F20" s="7" t="str">
         <f aca="false">'CERF Run'!Q3</f>
         <v>014B_C1000_1</v>
       </c>
-      <c r="I20" s="7" t="str">
+      <c r="G20" s="7" t="str">
         <f aca="false">'CERF Run'!R3</f>
         <v>014B_C1000_2</v>
       </c>
-      <c r="J20" s="7" t="str">
+      <c r="H20" s="7" t="str">
         <f aca="false">'CERF Run'!S3</f>
-        <v>100A_C1000_1</v>
-      </c>
-      <c r="K20" s="7" t="str">
+        <v>100_C1000_1</v>
+      </c>
+      <c r="I20" s="7" t="str">
         <f aca="false">'CERF Run'!T3</f>
-        <v>100A_C1000_2</v>
+        <v>100_C1000_2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B21" s="7" t="str">
-        <f aca="false">'CERF Run'!U3</f>
-        <v>100B_C1000_1</v>
-      </c>
-      <c r="C21" s="7" t="str">
-        <f aca="false">'CERF Run'!V3</f>
-        <v>100B_C1000_2</v>
-      </c>
-      <c r="D21" s="10" t="str">
+      <c r="B21" s="9" t="str">
         <f aca="false">'CERF Run'!C4</f>
         <v>PP_C2000_1</v>
       </c>
-      <c r="E21" s="10" t="str">
+      <c r="C21" s="9" t="str">
         <f aca="false">'CERF Run'!D4</f>
         <v>PP_C2000_2</v>
       </c>
-      <c r="F21" s="10" t="str">
+      <c r="D21" s="9" t="str">
         <f aca="false">'CERF Run'!E4</f>
         <v>HDPE_C2000_1</v>
       </c>
-      <c r="G21" s="10" t="str">
+      <c r="E21" s="9" t="str">
         <f aca="false">'CERF Run'!F4</f>
         <v>HDPE_C2000_2</v>
       </c>
-      <c r="H21" s="10" t="str">
+      <c r="F21" s="9" t="str">
         <f aca="false">'CERF Run'!G4</f>
         <v>005A_C2000_1</v>
       </c>
-      <c r="I21" s="10" t="str">
+      <c r="G21" s="9" t="str">
         <f aca="false">'CERF Run'!H4</f>
         <v>005A_C2000_2</v>
       </c>
-      <c r="J21" s="10" t="str">
+      <c r="H21" s="9" t="str">
         <f aca="false">'CERF Run'!I4</f>
         <v>005B_C2000_1</v>
       </c>
-      <c r="K21" s="10" t="str">
+      <c r="I21" s="9" t="str">
         <f aca="false">'CERF Run'!J4</f>
         <v>005B_C2000_2</v>
+      </c>
+      <c r="J21" s="9" t="str">
+        <f aca="false">'CERF Run'!K4</f>
+        <v>010A_C2000_1</v>
+      </c>
+      <c r="K21" s="9" t="str">
+        <f aca="false">'CERF Run'!L4</f>
+        <v>010A_C2000_2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B22" s="10" t="str">
-        <f aca="false">'CERF Run'!K4</f>
-        <v>010A_C2000_1</v>
-      </c>
-      <c r="C22" s="10" t="str">
-        <f aca="false">'CERF Run'!L4</f>
-        <v>010A_C2000_2</v>
-      </c>
-      <c r="D22" s="10" t="str">
+      <c r="B22" s="9" t="str">
         <f aca="false">'CERF Run'!M4</f>
         <v>010B_C2000_1</v>
       </c>
-      <c r="E22" s="10" t="str">
+      <c r="C22" s="9" t="str">
         <f aca="false">'CERF Run'!N4</f>
         <v>010B_C2000_2</v>
       </c>
-      <c r="F22" s="10" t="str">
+      <c r="D22" s="9" t="str">
         <f aca="false">'CERF Run'!O4</f>
         <v>014A_C2000_1</v>
       </c>
-      <c r="G22" s="10" t="str">
+      <c r="E22" s="9" t="str">
         <f aca="false">'CERF Run'!P4</f>
         <v>014A_C2000_2</v>
       </c>
-      <c r="H22" s="10" t="str">
+      <c r="F22" s="9" t="str">
         <f aca="false">'CERF Run'!Q4</f>
         <v>014B_C2000_1</v>
       </c>
-      <c r="I22" s="10" t="str">
+      <c r="G22" s="9" t="str">
         <f aca="false">'CERF Run'!R4</f>
         <v>014B_C2000_2</v>
       </c>
-      <c r="J22" s="10" t="str">
+      <c r="H22" s="9" t="str">
         <f aca="false">'CERF Run'!S4</f>
-        <v>100A_C2000_1</v>
-      </c>
-      <c r="K22" s="10" t="str">
+        <v>100_C2000_1</v>
+      </c>
+      <c r="I22" s="9" t="str">
         <f aca="false">'CERF Run'!T4</f>
-        <v>100A_C2000_2</v>
+        <v>100_C2000_2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B23" s="10" t="str">
-        <f aca="false">'CERF Run'!U4</f>
-        <v>100B_C2000_1</v>
-      </c>
-      <c r="C23" s="10" t="str">
-        <f aca="false">'CERF Run'!V4</f>
-        <v>100B_C2000_2</v>
-      </c>
-      <c r="D23" s="7" t="str">
+      <c r="B23" s="7" t="str">
         <f aca="false">'CERF Run'!C5</f>
         <v>PP_C200_1</v>
       </c>
-      <c r="E23" s="7" t="str">
+      <c r="C23" s="7" t="str">
         <f aca="false">'CERF Run'!D5</f>
         <v>PP_C200_2</v>
       </c>
-      <c r="F23" s="7" t="str">
+      <c r="D23" s="7" t="str">
         <f aca="false">'CERF Run'!E5</f>
         <v>HDPE_C200_1</v>
       </c>
-      <c r="G23" s="7" t="str">
+      <c r="E23" s="7" t="str">
         <f aca="false">'CERF Run'!F5</f>
         <v>HDPE_C200_2</v>
       </c>
-      <c r="H23" s="5" t="str">
+      <c r="F23" s="4" t="str">
         <f aca="false">'CERF Run'!C6</f>
         <v>PP_C400_1</v>
       </c>
-      <c r="I23" s="5" t="str">
+      <c r="G23" s="4" t="str">
         <f aca="false">'CERF Run'!D6</f>
         <v>PP_C400_2</v>
       </c>
-      <c r="J23" s="5" t="str">
+      <c r="H23" s="4" t="str">
         <f aca="false">'CERF Run'!E6</f>
         <v>HDPE_C400_1</v>
       </c>
-      <c r="K23" s="5" t="str">
+      <c r="I23" s="4" t="str">
         <f aca="false">'CERF Run'!F6</f>
         <v>HDPE_C400_2</v>
+      </c>
+      <c r="J23" s="9" t="str">
+        <f aca="false">'CERF Run'!C7</f>
+        <v>PP_C600_1</v>
+      </c>
+      <c r="K23" s="9" t="str">
+        <f aca="false">'CERF Run'!D7</f>
+        <v>PP_C600_2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B24" s="10" t="str">
-        <f aca="false">'CERF Run'!C7</f>
-        <v>PP_C600_1</v>
-      </c>
-      <c r="C24" s="10" t="str">
-        <f aca="false">'CERF Run'!D7</f>
-        <v>PP_C600_2</v>
-      </c>
-      <c r="D24" s="10" t="str">
+      <c r="B24" s="9" t="str">
         <f aca="false">'CERF Run'!E7</f>
         <v>HDPE_C600_1</v>
       </c>
-      <c r="E24" s="10" t="str">
+      <c r="C24" s="9" t="str">
         <f aca="false">'CERF Run'!F7</f>
         <v>HDPE_C600_2</v>
       </c>
-      <c r="F24" s="5" t="str">
+      <c r="D24" s="4" t="str">
         <f aca="false">'CERF Run'!C8</f>
         <v>PP_C800_1</v>
       </c>
-      <c r="G24" s="5" t="str">
+      <c r="E24" s="4" t="str">
         <f aca="false">'CERF Run'!D8</f>
         <v>PP_C800_2</v>
       </c>
-      <c r="H24" s="5" t="str">
+      <c r="F24" s="4" t="str">
         <f aca="false">'CERF Run'!E8</f>
         <v>HDPE_C800_1</v>
       </c>
-      <c r="I24" s="5" t="str">
+      <c r="G24" s="4" t="str">
         <f aca="false">'CERF Run'!F8</f>
         <v>HDPE_C800_2</v>
       </c>
@@ -2606,43 +2527,43 @@
       <c r="A26" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B26" s="9" t="str">
+      <c r="B26" s="10" t="str">
         <f aca="false">'Other Samples'!A2</f>
         <v>005A_Leach</v>
       </c>
-      <c r="C26" s="9" t="str">
+      <c r="C26" s="10" t="str">
         <f aca="false">'Other Samples'!B2</f>
         <v>005B_Leach</v>
       </c>
-      <c r="D26" s="9" t="str">
+      <c r="D26" s="10" t="str">
         <f aca="false">'Other Samples'!C2</f>
         <v>010A_Leach</v>
       </c>
-      <c r="E26" s="9" t="str">
+      <c r="E26" s="10" t="str">
         <f aca="false">'Other Samples'!D2</f>
         <v>010B_Leach</v>
       </c>
-      <c r="F26" s="9" t="str">
+      <c r="F26" s="10" t="str">
         <f aca="false">'Other Samples'!E2</f>
         <v>014A_Leach</v>
       </c>
-      <c r="G26" s="9" t="str">
+      <c r="G26" s="10" t="str">
         <f aca="false">'Other Samples'!F2</f>
         <v>014B_Leach</v>
       </c>
-      <c r="H26" s="9" t="str">
+      <c r="H26" s="10" t="str">
         <f aca="false">'Other Samples'!G2</f>
         <v>100_Leach</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>0</v>
@@ -2679,273 +2600,255 @@
       <c r="A31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="J31" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="K31" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>162</v>
-      </c>
+      <c r="B32" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>170</v>
+      <c r="B33" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>180</v>
+      <c r="B34" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>190</v>
+      <c r="B35" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>200</v>
+      <c r="B36" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>210</v>
+      <c r="B37" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
+      <c r="B38" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -2959,11 +2862,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2975,8 +2878,8 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2988,51 +2891,51 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">'CERF Run'!G2</f>
@@ -3081,14 +2984,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">StorageMatrix!K31</f>
         <v>010A_C100_2_REF</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">'CERF Run'!M2</f>
@@ -3133,7 +3036,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">'CERF Run'!R2</f>
@@ -3144,420 +3047,372 @@
         <v>014B_C100_2_REF</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="false">'CERF Run'!S2</f>
-        <v>100A_C100_1</v>
+        <v>100_C100_1</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">StorageMatrix!H32</f>
-        <v>100A_C100_1_REF</v>
+        <v>100_C100_1_REF</v>
       </c>
       <c r="G4" s="0" t="str">
         <f aca="false">'CERF Run'!T2</f>
-        <v>100A_C100_2</v>
+        <v>100_C100_2</v>
       </c>
       <c r="H4" s="0" t="str">
         <f aca="false">StorageMatrix!I32</f>
-        <v>100A_C100_2_REF</v>
-      </c>
-      <c r="I4" s="0" t="str">
-        <f aca="false">'CERF Run'!U2</f>
-        <v>100B_C100_1</v>
-      </c>
-      <c r="J4" s="0" t="str">
-        <f aca="false">StorageMatrix!J32</f>
-        <v>100B_C100_1_REF</v>
-      </c>
-      <c r="K4" s="0" t="str">
-        <f aca="false">'CERF Run'!V2</f>
-        <v>100B_C100_2</v>
-      </c>
-      <c r="L4" s="0" t="str">
-        <f aca="false">StorageMatrix!K32</f>
-        <v>100B_C100_2_REF</v>
-      </c>
-      <c r="M4" s="0" t="str">
+        <v>100_C100_2_REF</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" s="0" t="str">
         <f aca="false">'CERF Run'!G3</f>
         <v>005A_C1000_1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B5" s="0" t="str">
-        <f aca="false">StorageMatrix!H33</f>
+      <c r="C5" s="0" t="str">
+        <f aca="false">StorageMatrix!F33</f>
         <v>005A_C1000_1_REF</v>
       </c>
-      <c r="C5" s="0" t="str">
+      <c r="D5" s="0" t="str">
         <f aca="false">'CERF Run'!H3</f>
         <v>005A_C1000_2</v>
       </c>
-      <c r="D5" s="0" t="str">
-        <f aca="false">StorageMatrix!I33</f>
+      <c r="E5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">StorageMatrix!G33</f>
         <v>005A_C1000_2_REF</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="F5" s="0" t="str">
+      <c r="G5" s="0" t="str">
         <f aca="false">'CERF Run'!I3</f>
         <v>005B_C1000_1</v>
       </c>
-      <c r="G5" s="0" t="str">
-        <f aca="false">StorageMatrix!J33</f>
+      <c r="H5" s="0" t="str">
+        <f aca="false">StorageMatrix!H33</f>
         <v>005B_C1000_1_REF</v>
       </c>
-      <c r="H5" s="0" t="str">
+      <c r="I5" s="0" t="str">
         <f aca="false">'CERF Run'!J3</f>
         <v>005B_C1000_2</v>
       </c>
-      <c r="I5" s="0" t="str">
-        <f aca="false">StorageMatrix!K33</f>
+      <c r="J5" s="0" t="str">
+        <f aca="false">StorageMatrix!I33</f>
         <v>005B_C1000_2_REF</v>
       </c>
-      <c r="J5" s="0" t="str">
+      <c r="K5" s="0" t="str">
         <f aca="false">'CERF Run'!K3</f>
         <v>010A_C1000_1</v>
       </c>
-      <c r="K5" s="0" t="str">
-        <f aca="false">StorageMatrix!B34</f>
+      <c r="L5" s="0" t="str">
+        <f aca="false">StorageMatrix!J33</f>
         <v>010A_C1000_1_REF</v>
       </c>
-      <c r="L5" s="0" t="str">
+      <c r="M5" s="0" t="str">
         <f aca="false">'CERF Run'!L3</f>
         <v>010A_C1000_2</v>
       </c>
-      <c r="M5" s="0" t="str">
-        <f aca="false">StorageMatrix!C34</f>
-        <v>010A_C1000_2_REF</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B6" s="0" t="str">
+        <f aca="false">StorageMatrix!K33</f>
+        <v>010A_C1000_2_REF</v>
+      </c>
+      <c r="C6" s="0" t="str">
         <f aca="false">'CERF Run'!M3</f>
         <v>010B_C1000_1</v>
       </c>
-      <c r="C6" s="0" t="str">
-        <f aca="false">StorageMatrix!D34</f>
+      <c r="D6" s="0" t="str">
+        <f aca="false">StorageMatrix!B34</f>
         <v>010B_C1000_1_REF</v>
       </c>
-      <c r="D6" s="0" t="str">
+      <c r="E6" s="0" t="str">
         <f aca="false">'CERF Run'!N3</f>
         <v>010B_C1000_2</v>
       </c>
-      <c r="E6" s="0" t="str">
-        <f aca="false">StorageMatrix!E34</f>
+      <c r="F6" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">StorageMatrix!C34</f>
         <v>010B_C1000_2_REF</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="G6" s="0" t="str">
+      <c r="H6" s="0" t="str">
         <f aca="false">'CERF Run'!O3</f>
         <v>014A_C1000_1</v>
       </c>
-      <c r="H6" s="0" t="str">
-        <f aca="false">StorageMatrix!F34</f>
+      <c r="I6" s="0" t="str">
+        <f aca="false">StorageMatrix!D34</f>
         <v>014A_C1000_1_REF</v>
       </c>
-      <c r="I6" s="0" t="str">
+      <c r="J6" s="0" t="str">
         <f aca="false">'CERF Run'!P3</f>
         <v>014A_C1000_2</v>
       </c>
-      <c r="J6" s="0" t="str">
-        <f aca="false">StorageMatrix!G34</f>
+      <c r="K6" s="0" t="str">
+        <f aca="false">StorageMatrix!E34</f>
         <v>014A_C1000_2_REF</v>
       </c>
-      <c r="K6" s="0" t="str">
+      <c r="L6" s="0" t="str">
         <f aca="false">'CERF Run'!Q3</f>
         <v>014B_C1000_1</v>
       </c>
-      <c r="L6" s="0" t="str">
-        <f aca="false">StorageMatrix!H34</f>
+      <c r="M6" s="0" t="str">
+        <f aca="false">StorageMatrix!F34</f>
         <v>014B_C1000_1_REF</v>
       </c>
-      <c r="M6" s="0" t="str">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="0" t="str">
         <f aca="false">'CERF Run'!R3</f>
         <v>014B_C1000_2</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B7" s="0" t="str">
+      <c r="C7" s="0" t="str">
+        <f aca="false">StorageMatrix!G34</f>
+        <v>014B_C1000_2_REF</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">'CERF Run'!S3</f>
+        <v>100_C1000_1</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">StorageMatrix!H34</f>
+        <v>100_C1000_1_REF</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">'CERF Run'!T3</f>
+        <v>100_C1000_2</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" s="0" t="str">
         <f aca="false">StorageMatrix!I34</f>
-        <v>014B_C1000_2_REF</v>
-      </c>
-      <c r="C7" s="0" t="str">
-        <f aca="false">'CERF Run'!S3</f>
-        <v>100A_C1000_1</v>
-      </c>
-      <c r="D7" s="0" t="str">
-        <f aca="false">StorageMatrix!J34</f>
-        <v>100A_C1000_1_REF</v>
-      </c>
-      <c r="E7" s="0" t="str">
-        <f aca="false">'CERF Run'!T3</f>
-        <v>100A_C1000_2</v>
-      </c>
-      <c r="F7" s="0" t="str">
-        <f aca="false">StorageMatrix!K34</f>
-        <v>100A_C1000_2_REF</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="H7" s="0" t="str">
-        <f aca="false">'CERF Run'!U3</f>
-        <v>100B_C1000_1</v>
-      </c>
-      <c r="I7" s="0" t="str">
-        <f aca="false">StorageMatrix!B35</f>
-        <v>100B_C1000_1_REF</v>
-      </c>
-      <c r="J7" s="0" t="str">
-        <f aca="false">'CERF Run'!V3</f>
-        <v>100B_C1000_2</v>
-      </c>
-      <c r="K7" s="0" t="str">
-        <f aca="false">StorageMatrix!C35</f>
-        <v>100B_C1000_2_REF</v>
-      </c>
-      <c r="L7" s="0" t="str">
+        <v>100_C1000_2_REF</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="0" t="str">
         <f aca="false">'CERF Run'!G4</f>
         <v>005A_C2000_1</v>
       </c>
-      <c r="M7" s="0" t="str">
-        <f aca="false">StorageMatrix!H35</f>
+      <c r="C8" s="0" t="str">
+        <f aca="false">StorageMatrix!F35</f>
         <v>005A_C2000_1_REF</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B8" s="0" t="str">
+      <c r="D8" s="0" t="str">
         <f aca="false">'CERF Run'!H4</f>
         <v>005A_C2000_2</v>
       </c>
-      <c r="C8" s="0" t="str">
-        <f aca="false">StorageMatrix!I35</f>
+      <c r="E8" s="0" t="str">
+        <f aca="false">StorageMatrix!G35</f>
         <v>005A_C2000_2_REF</v>
       </c>
-      <c r="D8" s="0" t="str">
+      <c r="F8" s="0" t="str">
         <f aca="false">'CERF Run'!I4</f>
         <v>005B_C2000_1</v>
       </c>
-      <c r="E8" s="0" t="str">
-        <f aca="false">StorageMatrix!J35</f>
+      <c r="G8" s="0" t="str">
+        <f aca="false">StorageMatrix!H35</f>
         <v>005B_C2000_1_REF</v>
       </c>
-      <c r="F8" s="0" t="str">
+      <c r="H8" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="I8" s="0" t="str">
         <f aca="false">'CERF Run'!J4</f>
         <v>005B_C2000_2</v>
       </c>
-      <c r="G8" s="0" t="str">
-        <f aca="false">StorageMatrix!K35</f>
+      <c r="J8" s="0" t="str">
+        <f aca="false">StorageMatrix!I35</f>
         <v>005B_C2000_2_REF</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="I8" s="0" t="str">
+      <c r="K8" s="0" t="str">
         <f aca="false">'CERF Run'!K4</f>
         <v>010A_C2000_1</v>
       </c>
-      <c r="J8" s="0" t="str">
-        <f aca="false">StorageMatrix!B36</f>
+      <c r="L8" s="0" t="str">
+        <f aca="false">StorageMatrix!J35</f>
         <v>010A_C2000_1_REF</v>
       </c>
-      <c r="K8" s="0" t="str">
+      <c r="M8" s="0" t="str">
         <f aca="false">'CERF Run'!L4</f>
         <v>010A_C2000_2</v>
       </c>
-      <c r="L8" s="0" t="str">
-        <f aca="false">StorageMatrix!C36</f>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">StorageMatrix!K35</f>
         <v>010A_C2000_2_REF</v>
       </c>
-      <c r="M8" s="0" t="str">
+      <c r="C9" s="0" t="str">
         <f aca="false">'CERF Run'!M4</f>
         <v>010B_C2000_1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B9" s="0" t="str">
-        <f aca="false">StorageMatrix!D36</f>
+      <c r="D9" s="0" t="str">
+        <f aca="false">StorageMatrix!B36</f>
         <v>010B_C2000_1_REF</v>
       </c>
-      <c r="C9" s="0" t="str">
+      <c r="E9" s="0" t="str">
         <f aca="false">'CERF Run'!N4</f>
         <v>010B_C2000_2</v>
       </c>
-      <c r="D9" s="0" t="str">
-        <f aca="false">StorageMatrix!E36</f>
+      <c r="F9" s="0" t="str">
+        <f aca="false">StorageMatrix!C36</f>
         <v>010B_C2000_2_REF</v>
       </c>
-      <c r="E9" s="0" t="str">
+      <c r="G9" s="0" t="str">
         <f aca="false">'CERF Run'!O4</f>
         <v>014A_C2000_1</v>
       </c>
-      <c r="F9" s="0" t="str">
-        <f aca="false">StorageMatrix!F36</f>
+      <c r="H9" s="0" t="str">
+        <f aca="false">StorageMatrix!D36</f>
         <v>014A_C2000_1_REF</v>
       </c>
-      <c r="G9" s="0" t="str">
+      <c r="I9" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="J9" s="0" t="str">
         <f aca="false">'CERF Run'!P4</f>
         <v>014A_C2000_2</v>
       </c>
-      <c r="H9" s="0" t="str">
-        <f aca="false">StorageMatrix!G36</f>
+      <c r="K9" s="0" t="str">
+        <f aca="false">StorageMatrix!E36</f>
         <v>014A_C2000_2_REF</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="J9" s="0" t="str">
+      <c r="L9" s="0" t="str">
         <f aca="false">'CERF Run'!Q4</f>
         <v>014B_C2000_1</v>
       </c>
-      <c r="K9" s="0" t="str">
-        <f aca="false">StorageMatrix!H36</f>
+      <c r="M9" s="0" t="str">
+        <f aca="false">StorageMatrix!F36</f>
         <v>014B_C2000_1_REF</v>
       </c>
-      <c r="L9" s="0" t="str">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" s="0" t="str">
         <f aca="false">'CERF Run'!R4</f>
         <v>014B_C2000_2</v>
       </c>
-      <c r="M9" s="0" t="str">
+      <c r="C10" s="0" t="str">
+        <f aca="false">StorageMatrix!G36</f>
+        <v>014B_C2000_2_REF</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'CERF Run'!S4</f>
+        <v>100_C2000_1</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">StorageMatrix!H36</f>
+        <v>100_C2000_1_REF</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'CERF Run'!T4</f>
+        <v>100_C2000_2</v>
+      </c>
+      <c r="G10" s="0" t="str">
         <f aca="false">StorageMatrix!I36</f>
-        <v>014B_C2000_2_REF</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B10" s="0" t="str">
-        <f aca="false">'CERF Run'!S4</f>
-        <v>100A_C2000_1</v>
-      </c>
-      <c r="C10" s="0" t="str">
-        <f aca="false">StorageMatrix!J36</f>
-        <v>100A_C2000_1_REF</v>
-      </c>
-      <c r="D10" s="0" t="str">
-        <f aca="false">'CERF Run'!T4</f>
-        <v>100A_C2000_2</v>
-      </c>
-      <c r="E10" s="0" t="str">
-        <f aca="false">StorageMatrix!K36</f>
-        <v>100A_C2000_2_REF</v>
-      </c>
-      <c r="F10" s="0" t="str">
-        <f aca="false">'CERF Run'!U4</f>
-        <v>100B_C2000_1</v>
-      </c>
-      <c r="G10" s="0" t="str">
-        <f aca="false">StorageMatrix!B37</f>
-        <v>100B_C2000_1_REF</v>
-      </c>
-      <c r="H10" s="0" t="str">
-        <f aca="false">'CERF Run'!V4</f>
-        <v>100B_C2000_2</v>
-      </c>
-      <c r="I10" s="0" t="str">
-        <f aca="false">StorageMatrix!C37</f>
-        <v>100B_C2000_2_REF</v>
+        <v>100_C2000_2_REF</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>